<commit_message>
Update NED to search from a dictionary and add another version of NED using FAISS
</commit_message>
<xml_diff>
--- a/lib/abbreviation.xlsx
+++ b/lib/abbreviation.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphRAG\lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\NCKH\New\Graph_RAG\GraphRAG\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20801647-3C11-4FAB-A645-04D0A8F026F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{7DC9CFCB-2F20-244A-AA77-A9B5EFB544E6}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="13905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="120">
   <si>
     <t>ký túc xá</t>
   </si>
@@ -85,9 +84,6 @@
     <t>điểm trung bình chung học kỳ</t>
   </si>
   <si>
-    <t>điểm chung bình chung năm học</t>
-  </si>
-  <si>
     <t>thời khoá biểu</t>
   </si>
   <si>
@@ -238,9 +234,6 @@
     <t>chương trình chất lượng cao</t>
   </si>
   <si>
-    <t>p. ctsv</t>
-  </si>
-  <si>
     <t>Phòng Công tác Sinh viên</t>
   </si>
   <si>
@@ -305,12 +298,108 @@
   </si>
   <si>
     <t>báo cáo</t>
+  </si>
+  <si>
+    <t>bgh</t>
+  </si>
+  <si>
+    <t>Ban giám hiệu</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>Mác-Lênin</t>
+  </si>
+  <si>
+    <t>nckh</t>
+  </si>
+  <si>
+    <t>Nghiên cứu khoa học</t>
+  </si>
+  <si>
+    <t>nqhđt</t>
+  </si>
+  <si>
+    <t>Nghị Quyết Hội Đồng Trường</t>
+  </si>
+  <si>
+    <t>nđcp</t>
+  </si>
+  <si>
+    <t>Nghị định Chính Phủ</t>
+  </si>
+  <si>
+    <t>pđt</t>
+  </si>
+  <si>
+    <t>Phòng Đào Tạo</t>
+  </si>
+  <si>
+    <t>ttbgdđt</t>
+  </si>
+  <si>
+    <t>Thông tư Bộ Giáo dục và Đào tạo</t>
+  </si>
+  <si>
+    <t>ttbgdđtblđtbxh</t>
+  </si>
+  <si>
+    <t>Thông tư Bộ Giáo dục và Đào tạo, Bộ Lao động, Thương binh và Xã hội</t>
+  </si>
+  <si>
+    <t>vcnlđ</t>
+  </si>
+  <si>
+    <t>viên chức người lao động</t>
+  </si>
+  <si>
+    <t>đtbhk</t>
+  </si>
+  <si>
+    <t>điểm trung bình học kì</t>
+  </si>
+  <si>
+    <t>điểm trung bình chung năm học</t>
+  </si>
+  <si>
+    <t>ctđt ctclc</t>
+  </si>
+  <si>
+    <t>chương trình đào tạo chương trình chất lượng cao</t>
+  </si>
+  <si>
+    <t>ktxb</t>
+  </si>
+  <si>
+    <t>ký túc xá B</t>
+  </si>
+  <si>
+    <t>p.ctsv</t>
+  </si>
+  <si>
+    <t>p.htqt</t>
+  </si>
+  <si>
+    <t>Phòng Hợp tác Quốc tế</t>
+  </si>
+  <si>
+    <t>ttltbgdđtblđtbxh</t>
+  </si>
+  <si>
+    <t>Thông tư liên tịch Bộ Giáo dục và Đào tạo, Bộ Lao động, Thương binh và Xã hội</t>
+  </si>
+  <si>
+    <t>vbhnbgdđt</t>
+  </si>
+  <si>
+    <t>văn bản hợp nhất Bộ Giáo dục và Đào tạo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -655,388 +744,511 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F99DADB-5D27-6D4D-93EB-9727F161CE6F}">
-  <dimension ref="A1:B46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.625" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
       <c r="B9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>43</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B53" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>49</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B54" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>78</v>
-      </c>
-      <c r="B40" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" t="s">
-        <v>88</v>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>100</v>
+      </c>
+      <c r="B57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>102</v>
+      </c>
+      <c r="B59" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>104</v>
+      </c>
+      <c r="B60" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:B57">
+    <sortCondition ref="A56"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>